<commit_message>
Updated inventory list for next rig build
</commit_message>
<xml_diff>
--- a/partslist.xlsx
+++ b/partslist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anne\chipmunk_solo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132D807B-BBD5-42C9-B0E1-FE396EB54828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45060608-9EC6-49A6-B069-26325D1F18D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Walls and floor" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="156">
   <si>
     <t>Supplier</t>
   </si>
@@ -109,21 +109,6 @@
   </si>
   <si>
     <t>TR2</t>
-  </si>
-  <si>
-    <t>RLA 0600</t>
-  </si>
-  <si>
-    <t>Dovetail optical rail</t>
-  </si>
-  <si>
-    <t>Observer side view camera adjustment</t>
-  </si>
-  <si>
-    <t>RC1</t>
-  </si>
-  <si>
-    <t>Dovetail carrier, 1/4''</t>
   </si>
   <si>
     <t>Attaching dovetail optical rail to floor and 2'' post to dovetail carrier</t>
@@ -181,9 +166,6 @@
     <t>B07QF1VRPB</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>(Adapter with External M27 x 0.5 Threads and Internal SM1 Threads</t>
   </si>
   <si>
@@ -259,9 +241,6 @@
     <t>Grainger</t>
   </si>
   <si>
-    <t>3XYN9</t>
-  </si>
-  <si>
     <t>Haxagonal nylon standoff for 8/32 screws, pack of 10</t>
   </si>
   <si>
@@ -295,9 +274,6 @@
     <t>To attach PCB above the spacer plate</t>
   </si>
   <si>
-    <t>Haxagonal nylon standoff 0.5'' for 8/32 screws, pack of 10</t>
-  </si>
-  <si>
     <t>Spacer between the plate holding LED flashboards and the translucent white window in the back wall of the demonstrator</t>
   </si>
   <si>
@@ -308,66 +284,6 @@
   </si>
   <si>
     <t>Extract the other LED array for the stimulus presentation</t>
-  </si>
-  <si>
-    <t>Teensy 3.2</t>
-  </si>
-  <si>
-    <t>Adafruit</t>
-  </si>
-  <si>
-    <t>Control of the beam break for the observer deck</t>
-  </si>
-  <si>
-    <t>P1609</t>
-  </si>
-  <si>
-    <t>Perma-proto half-sized breadboard</t>
-  </si>
-  <si>
-    <t>Bread board for observer deck control</t>
-  </si>
-  <si>
-    <t>Teensy shield</t>
-  </si>
-  <si>
-    <t>Connect teensy to Bpod</t>
-  </si>
-  <si>
-    <t>3 mm infrared LED</t>
-  </si>
-  <si>
-    <t>Mouser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">696-OED-EL-8L </t>
-  </si>
-  <si>
-    <t>Observer deck beam break</t>
-  </si>
-  <si>
-    <t>3 mm photodiode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">710-1540031EC4590 </t>
-  </si>
-  <si>
-    <t>Resistor between 5V input and LED</t>
-  </si>
-  <si>
-    <t>Resistor between diode readout and ground</t>
-  </si>
-  <si>
-    <t>47 Ohm resistor, 1/4 W</t>
-  </si>
-  <si>
-    <t>1 MOhm resistor, 1/4 W</t>
-  </si>
-  <si>
-    <t>603-CFR-25JT-52-47R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">588-OK1055E-R52 </t>
   </si>
   <si>
     <t>Solenoid valve</t>
@@ -561,13 +477,34 @@
   </si>
   <si>
     <t>How many do we have?</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>sent to Anup for ordering</t>
+  </si>
+  <si>
+    <t>3XYL3</t>
+  </si>
+  <si>
+    <t>Haxagonal nylon standoff 0.25'' for 8/32 screws, pack of 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -582,6 +519,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -608,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -627,11 +571,97 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -941,10 +971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -957,11 +987,12 @@
     <col min="6" max="6" width="40.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -979,13 +1010,16 @@
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -998,244 +1032,231 @@
       <c r="E3">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4">
+        <v>4.88</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>8.7899999999999991</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D6">
-        <v>4.88</v>
+        <v>5.38</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
+        <v>21</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
-        <v>25</v>
+      <c r="C7" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="D7">
-        <v>8.7899999999999991</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>20</v>
+        <v>6.11</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
-        <v>26</v>
+      <c r="C8" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="D8">
-        <v>5.38</v>
-      </c>
-      <c r="E8">
-        <v>4</v>
+        <v>7.19</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D9">
-        <v>6.11</v>
+        <v>6.93</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D10">
-        <v>7.19</v>
+        <v>6.65</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11">
-        <v>6.93</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>66</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>60</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>18</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>59</v>
+      <c r="C12" t="s">
+        <v>23</v>
       </c>
       <c r="D12">
-        <v>6.65</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>66</v>
+        <v>10.050000000000001</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14">
-        <v>10.050000000000001</v>
-      </c>
-      <c r="E14">
-        <v>4</v>
-      </c>
-      <c r="F14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15">
-        <v>45.72</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16">
-        <v>26.94</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D18">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13">
         <v>36.99</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>135</v>
+      <c r="E13" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="m">
+      <formula>NOT(ISERROR(SEARCH("m",G1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="n">
+      <formula>NOT(ISERROR(SEARCH("n",G1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="y">
+      <formula>NOT(ISERROR(SEARCH("y",G1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
@@ -1247,10 +1268,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FA9598B-599D-42EB-A71C-CAB0F1B18FC1}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1267,7 +1288,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1285,18 +1306,18 @@
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C3">
         <v>1024</v>
@@ -1308,453 +1329,381 @@
         <v>1</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>79</v>
+      <c r="G5" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>80</v>
+        <v>74</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>13</v>
+        <v>75</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H8">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
+        <v>61</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9">
+        <v>8.27</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D10">
-        <v>8.27</v>
+        <v>3.59</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D11">
+        <v>2.92</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11">
-        <v>3.59</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="F11" s="6" t="s">
-        <v>86</v>
+        <v>80</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12">
-        <v>2.92</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>78</v>
+        <v>87</v>
+      </c>
+      <c r="C12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="3">
+        <v>2</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>87</v>
+        <v>89</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H12">
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" s="4">
+        <v>5.99</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14">
+        <v>76.3</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C14" s="3">
-        <v>2756</v>
-      </c>
-      <c r="D14">
-        <v>19.95</v>
-      </c>
-      <c r="E14" s="3">
-        <v>1</v>
-      </c>
-      <c r="F14" s="6" t="s">
+      <c r="B15" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="D15">
-        <v>4.5</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
+        <v>11.8</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16">
-        <v>1023</v>
+        <v>36</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="D16">
-        <v>32</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
+        <v>15.99</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17">
+        <v>9.99</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D17">
-        <v>0.4</v>
-      </c>
-      <c r="E17" s="3">
-        <v>1</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18">
-        <v>0.65</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
       <c r="E18" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>102</v>
+        <v>69</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="D19">
-        <v>0.1</v>
-      </c>
-      <c r="E19" s="3">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D20">
-        <v>0.13</v>
-      </c>
-      <c r="E20" s="3">
-        <v>1</v>
+        <v>36</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D20" s="5">
+        <v>7.78</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C22" t="s">
-        <v>114</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="3">
-        <v>4</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D23" s="4">
-        <v>5.99</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D24">
-        <v>76.3</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D25">
-        <v>11.8</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D26">
-        <v>15.99</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D27">
-        <v>9.99</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="E28" s="3">
-        <v>2</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D29">
-        <v>4</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="D30" s="5">
-        <v>7.78</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E36">
+        <v>66</v>
+      </c>
+      <c r="E26">
         <v>8</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>38</v>
+      <c r="F26" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="m">
+      <formula>NOT(ISERROR(SEARCH("m",G1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="n">
+      <formula>NOT(ISERROR(SEARCH("n",G1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="y">
+      <formula>NOT(ISERROR(SEARCH("y",G1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1763,8 +1712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1781,7 +1730,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1799,58 +1748,58 @@
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="E5" s="2">
         <v>1</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>173</v>
+        <v>145</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>172</v>
+        <v>144</v>
       </c>
       <c r="D6">
         <v>12.99</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>174</v>
+        <v>146</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D7">
         <v>6.99</v>
@@ -1859,18 +1808,18 @@
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
         <v>41</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
       </c>
       <c r="D8">
         <v>0.7</v>
@@ -1879,49 +1828,55 @@
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>88</v>
+        <v>155</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>76</v>
+        <v>154</v>
       </c>
       <c r="D9">
         <v>3.88</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>89</v>
+        <v>81</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E12" s="2">
         <v>1</v>
       </c>
+      <c r="G12" s="3" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D13">
         <v>5.99</v>
@@ -1930,18 +1885,18 @@
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D14">
         <v>3.99</v>
@@ -1950,7 +1905,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1981,7 +1936,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1999,21 +1954,21 @@
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="D3">
         <v>369</v>
@@ -2022,18 +1977,18 @@
         <v>3</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>139</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -2042,18 +1997,18 @@
         <v>3</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -2062,18 +2017,18 @@
         <v>3</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -2082,18 +2037,18 @@
         <v>3</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="D7">
         <v>132</v>
@@ -2102,38 +2057,38 @@
         <v>1</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>167</v>
+        <v>139</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>166</v>
+        <v>138</v>
       </c>
       <c r="D8" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>163</v>
+        <v>135</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>164</v>
+        <v>136</v>
       </c>
       <c r="D9">
         <v>52</v>
@@ -2142,27 +2097,27 @@
         <v>2</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>165</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D21">
         <v>21.86</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>